<commit_message>
Add test data and reST
</commit_message>
<xml_diff>
--- a/test/_res/sample.xlsx
+++ b/test/_res/sample.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkAyataka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sphinxcontrib-xlsxtable\test\_res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20745" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>A2</t>
     <phoneticPr fontId="1"/>
@@ -101,6 +102,22 @@
     <rPh sb="0" eb="3">
       <t>ニホンゴ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Item 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Item 2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -152,13 +169,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,4 +554,71 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="3"/>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add sample for start_row test
</commit_message>
<xml_diff>
--- a/test/_res/sample.xlsx
+++ b/test/_res/sample.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20745" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20745" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>A2</t>
     <phoneticPr fontId="1"/>
@@ -119,6 +120,87 @@
   <si>
     <t>Item 2</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>C8</t>
   </si>
 </sst>
 </file>
@@ -175,10 +257,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -487,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -511,7 +593,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -525,11 +607,11 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -575,7 +657,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B2">
@@ -583,19 +665,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B5">
@@ -603,14 +685,14 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -621,4 +703,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update test / sample
</commit_message>
<xml_diff>
--- a/test/_res/sample.xlsx
+++ b/test/_res/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>A2</t>
     <phoneticPr fontId="1"/>
@@ -201,6 +201,32 @@
   </si>
   <si>
     <t>C8</t>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
   </si>
 </sst>
 </file>
@@ -707,15 +733,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -725,8 +751,11 @@
       <c r="C1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -736,8 +765,11 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -747,8 +779,11 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -758,8 +793,11 @@
       <c r="C4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -769,8 +807,11 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -780,8 +821,11 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -791,8 +835,11 @@
       <c r="C7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -801,6 +848,9 @@
       </c>
       <c r="C8" t="s">
         <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>